<commit_message>
Added Search with SKU functionality
</commit_message>
<xml_diff>
--- a/LC_Workbook.xlsx
+++ b/LC_Workbook.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ValidUserItemsList" sheetId="1" r:id="rId1"/>
     <sheet name="GuestUserItemsList" sheetId="2" r:id="rId2"/>
     <sheet name="GuestUserBillingShippingAddress" sheetId="3" r:id="rId3"/>
+    <sheet name="SearchPanelList" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>CategoryName</t>
   </si>
@@ -137,13 +138,43 @@
   </si>
   <si>
     <t>123-456-7890</t>
+  </si>
+  <si>
+    <t>Colour</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Product_Names</t>
+  </si>
+  <si>
+    <t>Relavent_Names</t>
+  </si>
+  <si>
+    <t>070847038245</t>
+  </si>
+  <si>
+    <t>707510415408</t>
+  </si>
+  <si>
+    <t>412565696190</t>
+  </si>
+  <si>
+    <t>145627282829</t>
+  </si>
+  <si>
+    <t>SKU_Values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="000000000000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,16 +182,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -168,12 +213,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,7 +521,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +608,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,14 +618,14 @@
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -597,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,35 +679,35 @@
     <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -674,6 +738,75 @@
       </c>
       <c r="I2" t="s">
         <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new test cases for cart validation
</commit_message>
<xml_diff>
--- a/LC_Workbook.xlsx
+++ b/LC_Workbook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="897" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ValidUserStorePickupList" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="GuestUserItemsList" sheetId="2" r:id="rId3"/>
     <sheet name="GuestUserBillingShippingAddress" sheetId="3" r:id="rId4"/>
     <sheet name="SearchPanelList" sheetId="4" r:id="rId5"/>
+    <sheet name="ShoppingCartSettingsList" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
   <si>
     <t>CategoryName</t>
   </si>
@@ -51,9 +52,6 @@
     <t>E-Cig</t>
   </si>
   <si>
-    <t>RED BULL</t>
-  </si>
-  <si>
     <t>BRANDY</t>
   </si>
   <si>
@@ -175,6 +173,45 @@
   </si>
   <si>
     <t>Delivery</t>
+  </si>
+  <si>
+    <t>WINE</t>
+  </si>
+  <si>
+    <t>Champagne</t>
+  </si>
+  <si>
+    <t>Freixenet Prosecco</t>
+  </si>
+  <si>
+    <t>wine</t>
+  </si>
+  <si>
+    <t>moscato</t>
+  </si>
+  <si>
+    <t>Vignaioli Moscato D'asti</t>
+  </si>
+  <si>
+    <t>Wine</t>
+  </si>
+  <si>
+    <t>syrah</t>
+  </si>
+  <si>
+    <t>SPELLBOUND PETITE SIRAH</t>
+  </si>
+  <si>
+    <t>RED-BULL</t>
+  </si>
+  <si>
+    <t>KING-EDWARD</t>
+  </si>
+  <si>
+    <t>Organic-and-Kosher</t>
+  </si>
+  <si>
+    <t>Schlink Haus Organic Riesling</t>
   </si>
 </sst>
 </file>
@@ -529,7 +566,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,14 +576,14 @@
     <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -555,10 +592,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -566,10 +603,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -577,10 +614,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -588,10 +625,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -599,10 +636,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -616,7 +653,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,14 +663,14 @@
     <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -642,10 +679,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -653,10 +690,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
         <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -693,13 +730,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -707,10 +744,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -723,7 +760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -743,63 +780,63 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>33</v>
-      </c>
-      <c r="G2" t="s">
-        <v>34</v>
       </c>
       <c r="H2">
         <v>43623</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -826,36 +863,36 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -865,4 +902,79 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>